<commit_message>
add some modification in ArthurSpreeTC
</commit_message>
<xml_diff>
--- a/ArthurSpreeTC.xlsx
+++ b/ArthurSpreeTC.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/arthur718/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B38E6B1-4BA8-224D-B041-D5F4D4CF8421}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A73CD64-C3D5-0044-8711-4BBA4F8C69E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{7D12A46B-CFED-3D47-8873-E5027268D736}"/>
+    <workbookView xWindow="760" yWindow="900" windowWidth="28040" windowHeight="17040" xr2:uid="{7D12A46B-CFED-3D47-8873-E5027268D736}"/>
   </bookViews>
   <sheets>
-    <sheet name="TC001" sheetId="1" r:id="rId1"/>
+    <sheet name="TestSuite" sheetId="2" r:id="rId1"/>
+    <sheet name="TC001" sheetId="1" r:id="rId2"/>
+    <sheet name="TC002" sheetId="3" r:id="rId3"/>
+    <sheet name="TC003" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Steps</t>
   </si>
@@ -82,13 +85,70 @@
   </si>
   <si>
     <t>shiftqa01@gmail.com</t>
+  </si>
+  <si>
+    <t>TestScriptName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>ValidUserWithValidPassowrd</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>InvalidUserWithValidPassowrd</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>ValidUserWithinValidPassowrd</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>LoginPage.ErrorMessage</t>
+  </si>
+  <si>
+    <t>Invalid email or password.</t>
+  </si>
+  <si>
+    <t>shiftqa01xxx@gmail.com</t>
+  </si>
+  <si>
+    <t>Invalid email or password.XXX</t>
+  </si>
+  <si>
+    <t>HomePage.LogOut</t>
+  </si>
+  <si>
+    <t>Signed out successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,8 +162,24 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +189,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,10 +223,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -164,9 +247,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,11 +570,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EAFD59-484F-4040-A1EC-0C90EE41B366}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6150D95-5BB6-1547-9208-637C4B99F88C}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EAFD59-484F-4040-A1EC-0C90EE41B366}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,7 +707,7 @@
       <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -554,7 +721,7 @@
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -596,7 +763,279 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="16">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC86FD9-BFD2-564A-BDEC-F02FB414411D}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{214AE1C5-B344-3642-90F2-4C1D0A3ABCB6}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{2CCC19DF-7FE7-5E4C-B77E-BA04C4A68C59}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F022092E-4DCE-6644-9AF0-60B87C40CA94}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{98B95D1F-CE29-D949-A1ED-C0878180BD18}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{0CD6E9E5-767D-9441-9B17-B06C2E8E2EE2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>